<commit_message>
Removed fetal deaths before PNC encounter.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion07_Preeclampsia07.xlsx
+++ b/Parameters_Abortion07_Preeclampsia07.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65E445C-757F-9945-B681-D12592027BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763D72EF-90BB-3647-AC6D-6B2177CA9BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31900" yWindow="-660" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="31900" yWindow="-660" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="13" r:id="rId1"/>
@@ -46,19 +46,33 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={35C57926-D2D1-1E4D-B53B-E5E2E4FD75E7}</author>
+    <author>tc={781D2CE9-2320-E24A-B4CD-D415EAD7652C}</author>
     <author>tc={9A5BA4F2-D71D-6E40-92FE-646A717AC649}</author>
+    <author>tc={18D63495-01D6-0642-9BB2-9407F3435142}</author>
     <author>tc={AA203F26-57EB-FD4D-96A8-1E3EC58078F0}</author>
+    <author>tc={FB2D7D2D-7759-6F4E-BBDC-40B366DD516A}</author>
     <author>tc={BCDF96EB-9DF4-1E43-98E7-58F719177DD9}</author>
+    <author>tc={217B2CBD-A8A2-7649-AE06-E51F1325C5ED}</author>
     <author>tc={55A5B8CF-113A-584F-ABFB-262DB11F1536}</author>
+    <author>tc={FCE9BC3F-F1AA-EE44-8A2C-F4DCE32B9DE9}</author>
     <author>tc={20C24BD3-9274-DD49-BA6B-FAD26A6694BF}</author>
+    <author>tc={136188AF-5ABA-854F-8B38-88ED257E38DB}</author>
     <author>tc={C15EC358-19C4-624D-8519-888D9D36509A}</author>
+    <author>tc={087EB30E-D529-814C-9BE5-89C0BED73CE6}</author>
     <author>tc={DDBC1D8C-6502-5148-9760-A3D6248EE286}</author>
+    <author>tc={FE159CCB-C619-6344-B6C5-481E634D680B}</author>
     <author>tc={70D543EB-93BC-CD46-AD88-602A3D7EB00C}</author>
+    <author>tc={F3A1F740-3EE3-D04E-8B00-09E36C2B47F4}</author>
     <author>tc={2346C224-741D-FF43-8E6E-E465088EABEE}</author>
+    <author>tc={E039E581-77BB-2B45-A191-1091ACDD856D}</author>
     <author>tc={DA3B56D4-9145-A24D-B943-D5AAB2EEE929}</author>
+    <author>tc={F7F55EFA-D729-EE4E-B53E-DDF3A7CD7E0F}</author>
     <author>tc={2AA8F2D0-6E32-494D-B542-C416DAEFF657}</author>
+    <author>tc={EA114DEC-81B6-B24A-895A-AFFBF36140F4}</author>
     <author>tc={BA1965E4-CB1E-A446-858D-2C189AC85BC3}</author>
+    <author>tc={8A1BA2A5-D6A1-1B45-A850-1DE6A0663358}</author>
     <author>tc={266C3BF3-F32A-FA4C-ADA3-E234F64F1019}</author>
+    <author>tc={776C639E-08F4-2942-99F6-DB337B33BCF6}</author>
     <author>tc={73131F6C-4FDD-8242-81D0-C94D07ECA3E3}</author>
     <author>tc={A3BF7AB2-410D-5141-9C51-CD518C0D7571}</author>
     <author>tc={FC435F0F-04E0-0246-8288-D021C25AD0ED}</author>
@@ -72,9 +86,11 @@
     <author>tc={DB8D7BF8-7A77-C548-93AC-920263C47AE7}</author>
     <author>tc={F0934731-78BA-194A-B9CD-EC5F1F6C9CE0}</author>
     <author>tc={97E3E9D9-E3D7-4F43-B515-8C34E1CF5817}</author>
+    <author>tc={CF24B5A8-E800-3D45-A2C2-6648906D49B2}</author>
     <author>tc={22732877-B594-3A44-BC45-02143C03F17F}</author>
     <author>tc={EA6C2EE4-5812-B246-9332-1DE9E5ED6A26}</author>
     <author>tc={2C5EF934-2828-4B4A-9619-70709D64AE47}</author>
+    <author>tc={03E18539-D37D-2047-A130-CCA51965BB6F}</author>
     <author>tc={7B3AA43D-BF71-F649-BE1E-473187DEA264}</author>
   </authors>
   <commentList>
@@ -88,7 +104,17 @@
     Another resource. Though not the same population, this was helpful for understanding peaks</t>
       </text>
     </comment>
-    <comment ref="C2" authorId="1" shapeId="0" xr:uid="{9A5BA4F2-D71D-6E40-92FE-646A717AC649}">
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{781D2CE9-2320-E24A-B4CD-D415EAD7652C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://www.medicalnewstoday.com/articles/322634#miscarriage-rates-by-week
+Reply:
+    Another resource. Though not the same population, this was helpful for understanding peaks</t>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{9A5BA4F2-D71D-6E40-92FE-646A717AC649}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -98,7 +124,17 @@
     Brought it down further for computational efficiency to 0.1</t>
       </text>
     </comment>
-    <comment ref="C4" authorId="2" shapeId="0" xr:uid="{AA203F26-57EB-FD4D-96A8-1E3EC58078F0}">
+    <comment ref="F2" authorId="3" shapeId="0" xr:uid="{18D63495-01D6-0642-9BB2-9407F3435142}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.2. Same with gw 1
+Reply:
+    Brought it down further for computational efficiency to 0.1</t>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="4" shapeId="0" xr:uid="{AA203F26-57EB-FD4D-96A8-1E3EC58078F0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -108,7 +144,17 @@
     Lowered this even further to 0.05</t>
       </text>
     </comment>
-    <comment ref="C6" authorId="3" shapeId="0" xr:uid="{BCDF96EB-9DF4-1E43-98E7-58F719177DD9}">
+    <comment ref="F4" authorId="5" shapeId="0" xr:uid="{FB2D7D2D-7759-6F4E-BBDC-40B366DD516A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Lowered this slightly from 0.2 to 0.1 to improve sample size.
+Reply:
+    Lowered this even further to 0.05</t>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="6" shapeId="0" xr:uid="{BCDF96EB-9DF4-1E43-98E7-58F719177DD9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -116,7 +162,15 @@
     Was 0.05</t>
       </text>
     </comment>
-    <comment ref="C7" authorId="4" shapeId="0" xr:uid="{55A5B8CF-113A-584F-ABFB-262DB11F1536}">
+    <comment ref="F6" authorId="7" shapeId="0" xr:uid="{217B2CBD-A8A2-7649-AE06-E51F1325C5ED}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was 0.05</t>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="8" shapeId="0" xr:uid="{55A5B8CF-113A-584F-ABFB-262DB11F1536}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -124,7 +178,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C8" authorId="5" shapeId="0" xr:uid="{20C24BD3-9274-DD49-BA6B-FAD26A6694BF}">
+    <comment ref="F7" authorId="9" shapeId="0" xr:uid="{FCE9BC3F-F1AA-EE44-8A2C-F4DCE32B9DE9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -132,7 +186,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C9" authorId="6" shapeId="0" xr:uid="{C15EC358-19C4-624D-8519-888D9D36509A}">
+    <comment ref="C8" authorId="10" shapeId="0" xr:uid="{20C24BD3-9274-DD49-BA6B-FAD26A6694BF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -140,7 +194,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C10" authorId="7" shapeId="0" xr:uid="{DDBC1D8C-6502-5148-9760-A3D6248EE286}">
+    <comment ref="F8" authorId="11" shapeId="0" xr:uid="{136188AF-5ABA-854F-8B38-88ED257E38DB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -148,7 +202,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C11" authorId="8" shapeId="0" xr:uid="{70D543EB-93BC-CD46-AD88-602A3D7EB00C}">
+    <comment ref="C9" authorId="12" shapeId="0" xr:uid="{C15EC358-19C4-624D-8519-888D9D36509A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -156,7 +210,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C12" authorId="9" shapeId="0" xr:uid="{2346C224-741D-FF43-8E6E-E465088EABEE}">
+    <comment ref="F9" authorId="13" shapeId="0" xr:uid="{087EB30E-D529-814C-9BE5-89C0BED73CE6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -164,7 +218,7 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C13" authorId="10" shapeId="0" xr:uid="{DA3B56D4-9145-A24D-B943-D5AAB2EEE929}">
+    <comment ref="C10" authorId="14" shapeId="0" xr:uid="{DDBC1D8C-6502-5148-9760-A3D6248EE286}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -172,7 +226,63 @@
     Was 0.03</t>
       </text>
     </comment>
-    <comment ref="C20" authorId="11" shapeId="0" xr:uid="{2AA8F2D0-6E32-494D-B542-C416DAEFF657}">
+    <comment ref="F10" authorId="15" shapeId="0" xr:uid="{FE159CCB-C619-6344-B6C5-481E634D680B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was 0.03</t>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="16" shapeId="0" xr:uid="{70D543EB-93BC-CD46-AD88-602A3D7EB00C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was 0.03</t>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="17" shapeId="0" xr:uid="{F3A1F740-3EE3-D04E-8B00-09E36C2B47F4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was 0.03</t>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="18" shapeId="0" xr:uid="{2346C224-741D-FF43-8E6E-E465088EABEE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was 0.03</t>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="19" shapeId="0" xr:uid="{E039E581-77BB-2B45-A191-1091ACDD856D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was 0.03</t>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="20" shapeId="0" xr:uid="{DA3B56D4-9145-A24D-B943-D5AAB2EEE929}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was 0.03</t>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="21" shapeId="0" xr:uid="{F7F55EFA-D729-EE4E-B53E-DDF3A7CD7E0F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was 0.03</t>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="22" shapeId="0" xr:uid="{2AA8F2D0-6E32-494D-B542-C416DAEFF657}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -183,7 +293,18 @@
 Wanted to get the prevalence of stillbirth around 1-2%. In general, we see &lt;1% stillbirth in the MarketScan cohorts, though might be higher in a chronic hypertension population.</t>
       </text>
     </comment>
-    <comment ref="C21" authorId="12" shapeId="0" xr:uid="{BA1965E4-CB1E-A446-858D-2C189AC85BC3}">
+    <comment ref="F20" authorId="23" shapeId="0" xr:uid="{EA114DEC-81B6-B24A-895A-AFFBF36140F4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    All the 0.003s — https://stacks.cdc.gov/view/cdc/61387
+Reply:
+    This rate is per live births. Needs to be decreased. 
+Wanted to get the prevalence of stillbirth around 1-2%. In general, we see &lt;1% stillbirth in the MarketScan cohorts, though might be higher in a chronic hypertension population.</t>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="24" shapeId="0" xr:uid="{BA1965E4-CB1E-A446-858D-2C189AC85BC3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -191,7 +312,15 @@
     Originally 0.003s — https://stacks.cdc.gov/view/cdc/61387</t>
       </text>
     </comment>
-    <comment ref="C24" authorId="13" shapeId="0" xr:uid="{266C3BF3-F32A-FA4C-ADA3-E234F64F1019}">
+    <comment ref="F21" authorId="25" shapeId="0" xr:uid="{8A1BA2A5-D6A1-1B45-A850-1DE6A0663358}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally 0.003s — https://stacks.cdc.gov/view/cdc/61387</t>
+      </text>
+    </comment>
+    <comment ref="C24" authorId="26" shapeId="0" xr:uid="{266C3BF3-F32A-FA4C-ADA3-E234F64F1019}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -199,7 +328,15 @@
     Decreased risk after this point to reflect findings from this paper: https://journals.lww.com/greenjournal/fulltext/2015/12000/trends_in_stillbirth_by_gestational_age_in_the.5.aspx</t>
       </text>
     </comment>
-    <comment ref="D26" authorId="14" shapeId="0" xr:uid="{73131F6C-4FDD-8242-81D0-C94D07ECA3E3}">
+    <comment ref="F24" authorId="27" shapeId="0" xr:uid="{776C639E-08F4-2942-99F6-DB337B33BCF6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Decreased risk after this point to reflect findings from this paper: https://journals.lww.com/greenjournal/fulltext/2015/12000/trends_in_stillbirth_by_gestational_age_in_the.5.aspx</t>
+      </text>
+    </comment>
+    <comment ref="D26" authorId="28" shapeId="0" xr:uid="{73131F6C-4FDD-8242-81D0-C94D07ECA3E3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -209,7 +346,7 @@
     Previously 0.01</t>
       </text>
     </comment>
-    <comment ref="D27" authorId="15" shapeId="0" xr:uid="{A3BF7AB2-410D-5141-9C51-CD518C0D7571}">
+    <comment ref="D27" authorId="29" shapeId="0" xr:uid="{A3BF7AB2-410D-5141-9C51-CD518C0D7571}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -217,7 +354,7 @@
     Previously 0.01</t>
       </text>
     </comment>
-    <comment ref="D28" authorId="16" shapeId="0" xr:uid="{FC435F0F-04E0-0246-8288-D021C25AD0ED}">
+    <comment ref="D28" authorId="30" shapeId="0" xr:uid="{FC435F0F-04E0-0246-8288-D021C25AD0ED}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -225,7 +362,7 @@
     Previously 0.015</t>
       </text>
     </comment>
-    <comment ref="D29" authorId="17" shapeId="0" xr:uid="{B8929D9B-3F13-8D43-97FA-28992122F950}">
+    <comment ref="D29" authorId="31" shapeId="0" xr:uid="{B8929D9B-3F13-8D43-97FA-28992122F950}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -233,7 +370,7 @@
     Previously 0.015</t>
       </text>
     </comment>
-    <comment ref="D30" authorId="18" shapeId="0" xr:uid="{377E97A7-D950-D544-8EC5-6605C6A8C556}">
+    <comment ref="D30" authorId="32" shapeId="0" xr:uid="{377E97A7-D950-D544-8EC5-6605C6A8C556}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -241,7 +378,7 @@
     Previously 0.02</t>
       </text>
     </comment>
-    <comment ref="D31" authorId="19" shapeId="0" xr:uid="{9C3841F7-B168-E24B-A495-B612A936037C}">
+    <comment ref="D31" authorId="33" shapeId="0" xr:uid="{9C3841F7-B168-E24B-A495-B612A936037C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -249,7 +386,7 @@
     Previously 0.02</t>
       </text>
     </comment>
-    <comment ref="D32" authorId="20" shapeId="0" xr:uid="{852C6EAE-972D-594C-A185-FAD81F24BFAC}">
+    <comment ref="D32" authorId="34" shapeId="0" xr:uid="{852C6EAE-972D-594C-A185-FAD81F24BFAC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -257,7 +394,7 @@
     Previously 0.025</t>
       </text>
     </comment>
-    <comment ref="D33" authorId="21" shapeId="0" xr:uid="{C886D301-2ABB-0B44-8001-31BAF6B9FB99}">
+    <comment ref="D33" authorId="35" shapeId="0" xr:uid="{C886D301-2ABB-0B44-8001-31BAF6B9FB99}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -265,7 +402,7 @@
     Previously 0.03</t>
       </text>
     </comment>
-    <comment ref="D34" authorId="22" shapeId="0" xr:uid="{CCDC8F71-8200-9641-AEEF-2B20BAD612FE}">
+    <comment ref="D34" authorId="36" shapeId="0" xr:uid="{CCDC8F71-8200-9641-AEEF-2B20BAD612FE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -279,7 +416,7 @@
     Previously 0.15</t>
       </text>
     </comment>
-    <comment ref="D35" authorId="23" shapeId="0" xr:uid="{96162AFE-BCF7-FF46-8327-A20C0FF6288B}">
+    <comment ref="D35" authorId="37" shapeId="0" xr:uid="{96162AFE-BCF7-FF46-8327-A20C0FF6288B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -289,7 +426,7 @@
     Previously 0.03</t>
       </text>
     </comment>
-    <comment ref="D36" authorId="24" shapeId="0" xr:uid="{DB8D7BF8-7A77-C548-93AC-920263C47AE7}">
+    <comment ref="D36" authorId="38" shapeId="0" xr:uid="{DB8D7BF8-7A77-C548-93AC-920263C47AE7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -297,7 +434,7 @@
     Previously 0.06</t>
       </text>
     </comment>
-    <comment ref="C37" authorId="25" shapeId="0" xr:uid="{F0934731-78BA-194A-B9CD-EC5F1F6C9CE0}">
+    <comment ref="C37" authorId="39" shapeId="0" xr:uid="{F0934731-78BA-194A-B9CD-EC5F1F6C9CE0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -305,7 +442,7 @@
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</t>
       </text>
     </comment>
-    <comment ref="D37" authorId="26" shapeId="0" xr:uid="{97E3E9D9-E3D7-4F43-B515-8C34E1CF5817}">
+    <comment ref="D37" authorId="40" shapeId="0" xr:uid="{97E3E9D9-E3D7-4F43-B515-8C34E1CF5817}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -317,7 +454,15 @@
     Previously 0.05</t>
       </text>
     </comment>
-    <comment ref="D38" authorId="27" shapeId="0" xr:uid="{22732877-B594-3A44-BC45-02143C03F17F}">
+    <comment ref="F37" authorId="41" shapeId="0" xr:uid="{CF24B5A8-E800-3D45-A2C2-6648906D49B2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</t>
+      </text>
+    </comment>
+    <comment ref="D38" authorId="42" shapeId="0" xr:uid="{22732877-B594-3A44-BC45-02143C03F17F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -327,7 +472,7 @@
     Previously 0.17</t>
       </text>
     </comment>
-    <comment ref="D40" authorId="28" shapeId="0" xr:uid="{EA6C2EE4-5812-B246-9332-1DE9E5ED6A26}">
+    <comment ref="D40" authorId="43" shapeId="0" xr:uid="{EA6C2EE4-5812-B246-9332-1DE9E5ED6A26}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -335,7 +480,7 @@
     Previously 0.7</t>
       </text>
     </comment>
-    <comment ref="C60" authorId="29" shapeId="0" xr:uid="{2C5EF934-2828-4B4A-9619-70709D64AE47}">
+    <comment ref="C60" authorId="44" shapeId="0" xr:uid="{2C5EF934-2828-4B4A-9619-70709D64AE47}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -343,7 +488,15 @@
     This corresponds to the outcome observed at GA from LMP = 20</t>
       </text>
     </comment>
-    <comment ref="D108" authorId="30" shapeId="0" xr:uid="{7B3AA43D-BF71-F649-BE1E-473187DEA264}">
+    <comment ref="F60" authorId="45" shapeId="0" xr:uid="{03E18539-D37D-2047-A130-CCA51965BB6F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This corresponds to the outcome observed at GA from LMP = 20</t>
+      </text>
+    </comment>
+    <comment ref="D108" authorId="46" shapeId="0" xr:uid="{7B3AA43D-BF71-F649-BE1E-473187DEA264}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -572,7 +725,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
   <si>
     <t>p_fetaldeath</t>
   </si>
@@ -1084,12 +1237,15 @@
   <si>
     <t>g+B21</t>
   </si>
+  <si>
+    <t>p_fetaldeath_next_orig</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1140,6 +1296,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1597,10 +1759,22 @@
   <threadedComment ref="C1" dT="2024-06-21T20:36:49.49" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{734DA564-C48C-1448-9491-4E7030EC4887}" parentId="{35C57926-D2D1-1E4D-B53B-E5E2E4FD75E7}">
     <text>Another resource. Though not the same population, this was helpful for understanding peaks</text>
   </threadedComment>
+  <threadedComment ref="F1" dT="2023-10-20T20:28:15.91" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{781D2CE9-2320-E24A-B4CD-D415EAD7652C}">
+    <text>https://www.medicalnewstoday.com/articles/322634#miscarriage-rates-by-week</text>
+  </threadedComment>
+  <threadedComment ref="F1" dT="2024-06-21T20:36:49.49" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{A2122727-5C9A-B143-8F92-0FA07367EA2F}" parentId="{781D2CE9-2320-E24A-B4CD-D415EAD7652C}">
+    <text>Another resource. Though not the same population, this was helpful for understanding peaks</text>
+  </threadedComment>
   <threadedComment ref="C2" dT="2023-11-27T01:39:00.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{9A5BA4F2-D71D-6E40-92FE-646A717AC649}">
     <text>Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.2. Same with gw 1</text>
   </threadedComment>
   <threadedComment ref="C2" dT="2024-06-21T15:12:38.33" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{87CC0FEB-BD02-B441-89D9-2305B545E9B1}" parentId="{9A5BA4F2-D71D-6E40-92FE-646A717AC649}">
+    <text>Brought it down further for computational efficiency to 0.1</text>
+  </threadedComment>
+  <threadedComment ref="F2" dT="2023-11-27T01:39:00.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{18D63495-01D6-0642-9BB2-9407F3435142}">
+    <text>Originally had this as 0.5, but it was really high and lots of people not included in trial. Brought this down to 0.2. Same with gw 1</text>
+  </threadedComment>
+  <threadedComment ref="F2" dT="2024-06-21T15:12:38.33" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{04C43599-B7AF-FE4C-A321-E93F9483751B}" parentId="{18D63495-01D6-0642-9BB2-9407F3435142}">
     <text>Brought it down further for computational efficiency to 0.1</text>
   </threadedComment>
   <threadedComment ref="C4" dT="2023-11-27T01:41:40.99" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{AA203F26-57EB-FD4D-96A8-1E3EC58078F0}">
@@ -1609,28 +1783,58 @@
   <threadedComment ref="C4" dT="2024-07-05T19:53:57.22" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{8296E04E-70A2-DB43-B659-4C2DE60CCFB5}" parentId="{AA203F26-57EB-FD4D-96A8-1E3EC58078F0}">
     <text>Lowered this even further to 0.05</text>
   </threadedComment>
+  <threadedComment ref="F4" dT="2023-11-27T01:41:40.99" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{FB2D7D2D-7759-6F4E-BBDC-40B366DD516A}">
+    <text>Lowered this slightly from 0.2 to 0.1 to improve sample size.</text>
+  </threadedComment>
+  <threadedComment ref="F4" dT="2024-07-05T19:53:57.22" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{66581269-252C-254B-979F-116D036CEF06}" parentId="{FB2D7D2D-7759-6F4E-BBDC-40B366DD516A}">
+    <text>Lowered this even further to 0.05</text>
+  </threadedComment>
   <threadedComment ref="C6" dT="2024-06-21T18:59:28.37" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{BCDF96EB-9DF4-1E43-98E7-58F719177DD9}">
+    <text>Was 0.05</text>
+  </threadedComment>
+  <threadedComment ref="F6" dT="2024-06-21T18:59:28.37" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{217B2CBD-A8A2-7649-AE06-E51F1325C5ED}">
     <text>Was 0.05</text>
   </threadedComment>
   <threadedComment ref="C7" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{55A5B8CF-113A-584F-ABFB-262DB11F1536}">
     <text>Was 0.03</text>
   </threadedComment>
+  <threadedComment ref="F7" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{FCE9BC3F-F1AA-EE44-8A2C-F4DCE32B9DE9}">
+    <text>Was 0.03</text>
+  </threadedComment>
   <threadedComment ref="C8" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{20C24BD3-9274-DD49-BA6B-FAD26A6694BF}">
+    <text>Was 0.03</text>
+  </threadedComment>
+  <threadedComment ref="F8" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{136188AF-5ABA-854F-8B38-88ED257E38DB}">
     <text>Was 0.03</text>
   </threadedComment>
   <threadedComment ref="C9" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{C15EC358-19C4-624D-8519-888D9D36509A}">
     <text>Was 0.03</text>
   </threadedComment>
+  <threadedComment ref="F9" dT="2024-06-21T19:00:32.48" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{087EB30E-D529-814C-9BE5-89C0BED73CE6}">
+    <text>Was 0.03</text>
+  </threadedComment>
   <threadedComment ref="C10" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{DDBC1D8C-6502-5148-9760-A3D6248EE286}">
+    <text>Was 0.03</text>
+  </threadedComment>
+  <threadedComment ref="F10" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{FE159CCB-C619-6344-B6C5-481E634D680B}">
     <text>Was 0.03</text>
   </threadedComment>
   <threadedComment ref="C11" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{70D543EB-93BC-CD46-AD88-602A3D7EB00C}">
     <text>Was 0.03</text>
   </threadedComment>
+  <threadedComment ref="F11" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{F3A1F740-3EE3-D04E-8B00-09E36C2B47F4}">
+    <text>Was 0.03</text>
+  </threadedComment>
   <threadedComment ref="C12" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{2346C224-741D-FF43-8E6E-E465088EABEE}">
     <text>Was 0.03</text>
   </threadedComment>
+  <threadedComment ref="F12" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E039E581-77BB-2B45-A191-1091ACDD856D}">
+    <text>Was 0.03</text>
+  </threadedComment>
   <threadedComment ref="C13" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{DA3B56D4-9145-A24D-B943-D5AAB2EEE929}">
+    <text>Was 0.03</text>
+  </threadedComment>
+  <threadedComment ref="F13" dT="2024-06-21T19:00:51.59" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{F7F55EFA-D729-EE4E-B53E-DDF3A7CD7E0F}">
     <text>Was 0.03</text>
   </threadedComment>
   <threadedComment ref="C20" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{2AA8F2D0-6E32-494D-B542-C416DAEFF657}">
@@ -1640,10 +1844,29 @@
     <text>This rate is per live births. Needs to be decreased. 
 Wanted to get the prevalence of stillbirth around 1-2%. In general, we see &lt;1% stillbirth in the MarketScan cohorts, though might be higher in a chronic hypertension population.</text>
   </threadedComment>
+  <threadedComment ref="F20" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{EA114DEC-81B6-B24A-895A-AFFBF36140F4}">
+    <text>All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</text>
+  </threadedComment>
+  <threadedComment ref="F20" dT="2024-06-19T20:53:57.65" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{97456867-7F0F-AD42-8438-579554D435A8}" parentId="{EA114DEC-81B6-B24A-895A-AFFBF36140F4}">
+    <text>This rate is per live births. Needs to be decreased. 
+Wanted to get the prevalence of stillbirth around 1-2%. In general, we see &lt;1% stillbirth in the MarketScan cohorts, though might be higher in a chronic hypertension population.</text>
+  </threadedComment>
   <threadedComment ref="C21" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{BA1965E4-CB1E-A446-858D-2C189AC85BC3}">
     <text>Originally 0.003s — https://stacks.cdc.gov/view/cdc/61387</text>
   </threadedComment>
+  <threadedComment ref="F21" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{8A1BA2A5-D6A1-1B45-A850-1DE6A0663358}">
+    <text>Originally 0.003s — https://stacks.cdc.gov/view/cdc/61387</text>
+  </threadedComment>
   <threadedComment ref="C24" dT="2024-06-21T18:06:37.21" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{266C3BF3-F32A-FA4C-ADA3-E234F64F1019}">
+    <text>Decreased risk after this point to reflect findings from this paper: https://journals.lww.com/greenjournal/fulltext/2015/12000/trends_in_stillbirth_by_gestational_age_in_the.5.aspx</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>1471286569</xltc2:checksum>
+        <xltc2:hyperlink startIndex="69" length="111" url="https://journals.lww.com/greenjournal/fulltext/2015/12000/trends_in_stillbirth_by_gestational_age_in_the.5.aspx"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="F24" dT="2024-06-21T18:06:37.21" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{776C639E-08F4-2942-99F6-DB337B33BCF6}">
     <text>Decreased risk after this point to reflect findings from this paper: https://journals.lww.com/greenjournal/fulltext/2015/12000/trends_in_stillbirth_by_gestational_age_in_the.5.aspx</text>
     <extLst>
       <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
@@ -1712,6 +1935,9 @@
   <threadedComment ref="D37" dT="2024-07-12T13:50:56.67" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{9DCA148F-50FB-0949-9EF8-E60CF9728C79}" parentId="{97E3E9D9-E3D7-4F43-B515-8C34E1CF5817}">
     <text>Previously 0.05</text>
   </threadedComment>
+  <threadedComment ref="F37" dT="2023-10-20T20:29:33.53" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{CF24B5A8-E800-3D45-A2C2-6648906D49B2}">
+    <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</text>
+  </threadedComment>
   <threadedComment ref="D38" dT="2024-06-21T18:00:19.51" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{22732877-B594-3A44-BC45-02143C03F17F}">
     <text>Previously 0.35</text>
   </threadedComment>
@@ -1722,6 +1948,9 @@
     <text>Previously 0.7</text>
   </threadedComment>
   <threadedComment ref="C60" dT="2024-07-12T18:29:36.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{2C5EF934-2828-4B4A-9619-70709D64AE47}">
+    <text>This corresponds to the outcome observed at GA from LMP = 20</text>
+  </threadedComment>
+  <threadedComment ref="F60" dT="2024-07-12T18:29:36.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{03E18539-D37D-2047-A130-CCA51965BB6F}">
     <text>This corresponds to the outcome observed at GA from LMP = 20</text>
   </threadedComment>
   <threadedComment ref="D108" dT="2023-10-20T20:36:59.95" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{7B3AA43D-BF71-F649-BE1E-473187DEA264}">
@@ -1991,7 +2220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBAD042-1D8C-E044-AB59-2B80CE0D260D}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2138,10 +2367,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2150,10 +2379,10 @@
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2169,8 +2398,11 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -2178,17 +2410,20 @@
         <v>0</v>
       </c>
       <c r="C2" s="8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="8">
         <v>0</v>
       </c>
       <c r="E2" s="2">
         <f>1-D2-C2</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -2196,17 +2431,20 @@
         <v>1</v>
       </c>
       <c r="C3" s="8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
       </c>
       <c r="E3" s="2">
         <f>1-D3-C3</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -2214,17 +2452,20 @@
         <v>2</v>
       </c>
       <c r="C4" s="8">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D4" s="8">
         <v>0</v>
       </c>
       <c r="E4" s="2">
         <f>1-D4-C4</f>
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>0</v>
       </c>
@@ -2232,17 +2473,20 @@
         <v>3</v>
       </c>
       <c r="C5" s="8">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D5" s="8">
         <v>0</v>
       </c>
       <c r="E5" s="2">
         <f>1-D5-C5</f>
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -2250,17 +2494,20 @@
         <v>4</v>
       </c>
       <c r="C6" s="8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="8">
         <v>0</v>
       </c>
       <c r="E6" s="2">
         <f>1-D6-C6</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>0</v>
       </c>
@@ -2268,17 +2515,20 @@
         <v>5</v>
       </c>
       <c r="C7" s="8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="8">
         <v>0</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" ref="E7:E41" si="0">1-C7-D7</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>0</v>
       </c>
@@ -2286,17 +2536,20 @@
         <v>6</v>
       </c>
       <c r="C8" s="8">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="D8" s="8">
         <v>0</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>0</v>
       </c>
@@ -2313,8 +2566,11 @@
         <f t="shared" si="0"/>
         <v>0.91</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="8">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>0</v>
       </c>
@@ -2331,8 +2587,11 @@
         <f t="shared" si="0"/>
         <v>0.98499999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>0</v>
       </c>
@@ -2349,8 +2608,11 @@
         <f t="shared" si="0"/>
         <v>0.98499999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>0</v>
       </c>
@@ -2367,8 +2629,11 @@
         <f t="shared" si="0"/>
         <v>0.98499999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>0</v>
       </c>
@@ -2385,8 +2650,11 @@
         <f t="shared" si="0"/>
         <v>0.98499999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>0</v>
       </c>
@@ -2403,8 +2671,11 @@
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>0</v>
       </c>
@@ -2421,8 +2692,11 @@
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>0</v>
       </c>
@@ -2439,8 +2713,11 @@
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>0</v>
       </c>
@@ -2457,8 +2734,11 @@
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>0</v>
       </c>
@@ -2475,8 +2755,11 @@
         <f t="shared" si="0"/>
         <v>0.99919999999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="8">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>0</v>
       </c>
@@ -2493,8 +2776,11 @@
         <f t="shared" si="0"/>
         <v>0.99919999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="8">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>0</v>
       </c>
@@ -2511,8 +2797,11 @@
         <f t="shared" si="0"/>
         <v>0.99919999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="8">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>0</v>
       </c>
@@ -2529,8 +2818,11 @@
         <f t="shared" si="0"/>
         <v>0.99919999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="8">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>0</v>
       </c>
@@ -2547,8 +2839,11 @@
         <f t="shared" si="0"/>
         <v>0.99997499999999995</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="8">
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>0</v>
       </c>
@@ -2565,8 +2860,11 @@
         <f t="shared" si="0"/>
         <v>0.99998940000000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="8">
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>0</v>
       </c>
@@ -2583,8 +2881,11 @@
         <f t="shared" si="0"/>
         <v>0.99998940000000003</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="8">
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>0</v>
       </c>
@@ -2601,8 +2902,11 @@
         <f t="shared" si="0"/>
         <v>0.99998940000000003</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="8">
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>0</v>
       </c>
@@ -2619,8 +2923,11 @@
         <f t="shared" si="0"/>
         <v>0.99899939999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="8">
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>0</v>
       </c>
@@ -2637,8 +2944,11 @@
         <f t="shared" si="0"/>
         <v>0.99849940000000004</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="8">
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>0</v>
       </c>
@@ -2655,8 +2965,11 @@
         <f t="shared" si="0"/>
         <v>0.99819939999999996</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="8">
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>0</v>
       </c>
@@ -2673,8 +2986,11 @@
         <f t="shared" si="0"/>
         <v>0.99799400000000005</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="8">
+        <v>6.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>0</v>
       </c>
@@ -2691,8 +3007,11 @@
         <f t="shared" si="0"/>
         <v>0.99697499999999994</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="8">
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>0</v>
       </c>
@@ -2709,8 +3028,11 @@
         <f t="shared" si="0"/>
         <v>0.99497499999999994</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="8">
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>0</v>
       </c>
@@ -2727,8 +3049,11 @@
         <f t="shared" si="0"/>
         <v>0.99397499999999994</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="8">
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>0</v>
       </c>
@@ -2745,8 +3070,11 @@
         <f t="shared" si="0"/>
         <v>0.99185000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="8">
+        <v>1.4999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>0</v>
       </c>
@@ -2763,8 +3091,11 @@
         <f t="shared" si="0"/>
         <v>0.94964999999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="8">
+        <v>3.5E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>0</v>
       </c>
@@ -2781,8 +3112,11 @@
         <f t="shared" si="0"/>
         <v>0.91944999999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="8">
+        <v>5.5000000000000003E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>0</v>
       </c>
@@ -2799,8 +3133,11 @@
         <f t="shared" si="0"/>
         <v>0.64650000000000007</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="8">
+        <v>3.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>0</v>
       </c>
@@ -2817,8 +3154,11 @@
         <f t="shared" si="0"/>
         <v>0.59850000000000003</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="8">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>0</v>
       </c>
@@ -2835,8 +3175,11 @@
         <f t="shared" si="0"/>
         <v>0.2984</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="8">
+        <v>1.6000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>0</v>
       </c>
@@ -2853,8 +3196,11 @@
         <f t="shared" si="0"/>
         <v>0.29400000000000004</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>0</v>
       </c>
@@ -2871,8 +3217,11 @@
         <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>0</v>
       </c>
@@ -2889,8 +3238,11 @@
         <f t="shared" si="0"/>
         <v>0.10000000000000009</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>0</v>
       </c>
@@ -2907,8 +3259,11 @@
       <c r="E42" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>1</v>
       </c>
@@ -2917,7 +3272,7 @@
       </c>
       <c r="C43" s="3">
         <f>C2*SimParameters!B9</f>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="D43" s="3">
         <f>D2</f>
@@ -2925,10 +3280,14 @@
       </c>
       <c r="E43" s="3">
         <f>1-D43-C43</f>
-        <v>0.875</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <f>F2*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>1</v>
       </c>
@@ -2937,7 +3296,7 @@
       </c>
       <c r="C44" s="3">
         <f>C3*SimParameters!B9</f>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="D44" s="3">
         <f t="shared" ref="D44:D83" si="1">D3</f>
@@ -2945,10 +3304,14 @@
       </c>
       <c r="E44" s="3">
         <f>1-D44-C44</f>
-        <v>0.875</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F44" s="3">
+        <f>F3*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>1</v>
       </c>
@@ -2957,7 +3320,7 @@
       </c>
       <c r="C45" s="3">
         <f>C4*SimParameters!B9</f>
-        <v>6.25E-2</v>
+        <v>0</v>
       </c>
       <c r="D45" s="3">
         <f t="shared" si="1"/>
@@ -2965,10 +3328,14 @@
       </c>
       <c r="E45" s="3">
         <f>1-D45-C45</f>
-        <v>0.9375</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3">
+        <f>F4*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>1</v>
       </c>
@@ -2977,7 +3344,7 @@
       </c>
       <c r="C46" s="3">
         <f>C5*SimParameters!B9</f>
-        <v>6.25E-2</v>
+        <v>0</v>
       </c>
       <c r="D46" s="3">
         <f t="shared" si="1"/>
@@ -2985,10 +3352,14 @@
       </c>
       <c r="E46" s="3">
         <f>1-D46-C46</f>
-        <v>0.9375</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3">
+        <f>F5*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>1</v>
       </c>
@@ -2997,7 +3368,7 @@
       </c>
       <c r="C47" s="3">
         <f>C6*SimParameters!B9</f>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="D47" s="3">
         <f t="shared" si="1"/>
@@ -3005,10 +3376,14 @@
       </c>
       <c r="E47" s="3">
         <f>1-D47-C47</f>
-        <v>0.875</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
+        <f>F6*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>1</v>
       </c>
@@ -3017,7 +3392,7 @@
       </c>
       <c r="C48" s="3">
         <f>C7*SimParameters!B9</f>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="D48" s="3">
         <f t="shared" si="1"/>
@@ -3025,10 +3400,14 @@
       </c>
       <c r="E48" s="3">
         <f t="shared" ref="E48:E82" si="2">1-C48-D48</f>
-        <v>0.875</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3">
+        <f>F7*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>1</v>
       </c>
@@ -3037,7 +3416,7 @@
       </c>
       <c r="C49" s="3">
         <f>C8*SimParameters!B9</f>
-        <v>0.11249999999999999</v>
+        <v>0</v>
       </c>
       <c r="D49" s="3">
         <f t="shared" si="1"/>
@@ -3045,10 +3424,14 @@
       </c>
       <c r="E49" s="3">
         <f t="shared" si="2"/>
-        <v>0.88749999999999996</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3">
+        <f>F8*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>1</v>
       </c>
@@ -3067,8 +3450,12 @@
         <f t="shared" si="2"/>
         <v>0.88749999999999996</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="3">
+        <f>F9*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>1</v>
       </c>
@@ -3087,8 +3474,12 @@
         <f t="shared" si="2"/>
         <v>0.98124999999999996</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="3">
+        <f>F10*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>1</v>
       </c>
@@ -3107,8 +3498,12 @@
         <f t="shared" si="2"/>
         <v>0.98124999999999996</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="3">
+        <f>F11*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>1</v>
       </c>
@@ -3127,8 +3522,12 @@
         <f t="shared" si="2"/>
         <v>0.98124999999999996</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="3">
+        <f>F12*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>1</v>
       </c>
@@ -3147,8 +3546,12 @@
         <f t="shared" si="2"/>
         <v>0.98124999999999996</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="3">
+        <f>F13*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>1</v>
       </c>
@@ -3167,8 +3570,12 @@
         <f t="shared" si="2"/>
         <v>0.98750000000000004</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="3">
+        <f>F14*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>1</v>
       </c>
@@ -3187,8 +3594,12 @@
         <f t="shared" si="2"/>
         <v>0.98750000000000004</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="3">
+        <f>F15*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>1</v>
       </c>
@@ -3207,8 +3618,12 @@
         <f t="shared" si="2"/>
         <v>0.98750000000000004</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="3">
+        <f>F16*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>1</v>
       </c>
@@ -3227,8 +3642,12 @@
         <f t="shared" si="2"/>
         <v>0.98750000000000004</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="3">
+        <f>F17*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>1</v>
       </c>
@@ -3247,8 +3666,12 @@
         <f t="shared" si="2"/>
         <v>0.999</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="3">
+        <f>F18*SimParameters!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>1</v>
       </c>
@@ -3267,8 +3690,12 @@
         <f t="shared" si="2"/>
         <v>0.99919999999999998</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="3">
+        <f>F19</f>
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>1</v>
       </c>
@@ -3287,8 +3714,12 @@
         <f t="shared" si="2"/>
         <v>0.99919999999999998</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="3">
+        <f t="shared" ref="F61:F83" si="4">F20</f>
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>1</v>
       </c>
@@ -3307,8 +3738,12 @@
         <f t="shared" si="2"/>
         <v>0.99919999999999998</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="3">
+        <f t="shared" si="4"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>1</v>
       </c>
@@ -3327,8 +3762,12 @@
         <f t="shared" si="2"/>
         <v>0.99997499999999995</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="3">
+        <f t="shared" si="4"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>1</v>
       </c>
@@ -3347,8 +3786,12 @@
         <f t="shared" si="2"/>
         <v>0.99998940000000003</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" s="3">
+        <f t="shared" si="4"/>
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>1</v>
       </c>
@@ -3367,8 +3810,12 @@
         <f t="shared" si="2"/>
         <v>0.99998940000000003</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="3">
+        <f t="shared" si="4"/>
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>1</v>
       </c>
@@ -3387,8 +3834,12 @@
         <f t="shared" si="2"/>
         <v>0.99998940000000003</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="3">
+        <f t="shared" si="4"/>
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>1</v>
       </c>
@@ -3407,8 +3858,12 @@
         <f t="shared" si="2"/>
         <v>0.99899939999999998</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" s="3">
+        <f t="shared" si="4"/>
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>1</v>
       </c>
@@ -3427,8 +3882,12 @@
         <f t="shared" si="2"/>
         <v>0.99849940000000004</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="3">
+        <f t="shared" si="4"/>
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>1</v>
       </c>
@@ -3447,8 +3906,12 @@
         <f t="shared" si="2"/>
         <v>0.99819939999999996</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" s="3">
+        <f t="shared" si="4"/>
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>1</v>
       </c>
@@ -3467,8 +3930,12 @@
         <f t="shared" si="2"/>
         <v>0.99799400000000005</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="3">
+        <f t="shared" si="4"/>
+        <v>6.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>1</v>
       </c>
@@ -3487,8 +3954,12 @@
         <f t="shared" si="2"/>
         <v>0.99697499999999994</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" s="3">
+        <f t="shared" si="4"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>1</v>
       </c>
@@ -3507,8 +3978,12 @@
         <f t="shared" si="2"/>
         <v>0.99497499999999994</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="3">
+        <f t="shared" si="4"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>1</v>
       </c>
@@ -3527,8 +4002,12 @@
         <f t="shared" si="2"/>
         <v>0.99397499999999994</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" s="3">
+        <f t="shared" si="4"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>1</v>
       </c>
@@ -3547,8 +4026,12 @@
         <f t="shared" si="2"/>
         <v>0.99185000000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="3">
+        <f t="shared" si="4"/>
+        <v>1.4999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>1</v>
       </c>
@@ -3567,8 +4050,12 @@
         <f t="shared" si="2"/>
         <v>0.94964999999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" s="3">
+        <f t="shared" si="4"/>
+        <v>3.5E-4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>1</v>
       </c>
@@ -3587,8 +4074,12 @@
         <f t="shared" si="2"/>
         <v>0.91944999999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" s="3">
+        <f t="shared" si="4"/>
+        <v>5.5000000000000003E-4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>1</v>
       </c>
@@ -3607,8 +4098,12 @@
         <f t="shared" si="2"/>
         <v>0.64650000000000007</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" s="3">
+        <f t="shared" si="4"/>
+        <v>3.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>1</v>
       </c>
@@ -3627,8 +4122,12 @@
         <f t="shared" si="2"/>
         <v>0.59850000000000003</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="3">
+        <f t="shared" si="4"/>
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>1</v>
       </c>
@@ -3647,8 +4146,12 @@
         <f t="shared" si="2"/>
         <v>0.2984</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" s="3">
+        <f t="shared" si="4"/>
+        <v>1.6000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>1</v>
       </c>
@@ -3667,8 +4170,12 @@
         <f t="shared" si="2"/>
         <v>0.29400000000000004</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" s="3">
+        <f t="shared" si="4"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>1</v>
       </c>
@@ -3687,8 +4194,12 @@
         <f t="shared" si="2"/>
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81" s="3">
+        <f t="shared" si="4"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>1</v>
       </c>
@@ -3707,8 +4218,12 @@
         <f t="shared" si="2"/>
         <v>0.10000000000000009</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82" s="3">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>1</v>
       </c>
@@ -3726,8 +4241,12 @@
       <c r="E83" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83" s="3">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>2</v>
       </c>
@@ -3736,7 +4255,7 @@
       </c>
       <c r="C84" s="4">
         <f>C2*SimParameters!B10</f>
-        <v>0.15000000000000002</v>
+        <v>0</v>
       </c>
       <c r="D84" s="4">
         <f>D2</f>
@@ -3744,10 +4263,14 @@
       </c>
       <c r="E84" s="4">
         <f>1-D84-C84</f>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F84" s="4">
+        <f>F2*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>2</v>
       </c>
@@ -3756,18 +4279,22 @@
       </c>
       <c r="C85" s="4">
         <f>C3*SimParameters!B10</f>
-        <v>0.15000000000000002</v>
+        <v>0</v>
       </c>
       <c r="D85" s="4">
-        <f t="shared" ref="D85:D124" si="4">D3</f>
+        <f t="shared" ref="D85:D124" si="5">D3</f>
         <v>0</v>
       </c>
       <c r="E85" s="4">
         <f>1-D85-C85</f>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F85" s="4">
+        <f>F3*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>2</v>
       </c>
@@ -3776,18 +4303,22 @@
       </c>
       <c r="C86" s="4">
         <f>C4*SimParameters!B10</f>
-        <v>7.5000000000000011E-2</v>
+        <v>0</v>
       </c>
       <c r="D86" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E86" s="4">
         <f>1-D86-C86</f>
-        <v>0.92500000000000004</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F86" s="4">
+        <f>F4*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>2</v>
       </c>
@@ -3796,18 +4327,22 @@
       </c>
       <c r="C87" s="4">
         <f>C5*SimParameters!B10</f>
-        <v>7.5000000000000011E-2</v>
+        <v>0</v>
       </c>
       <c r="D87" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E87" s="4">
         <f>1-D87-C87</f>
-        <v>0.92500000000000004</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F87" s="4">
+        <f>F5*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>2</v>
       </c>
@@ -3816,18 +4351,22 @@
       </c>
       <c r="C88" s="4">
         <f>C6*SimParameters!B10</f>
-        <v>0.15000000000000002</v>
+        <v>0</v>
       </c>
       <c r="D88" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E88" s="4">
         <f>1-D88-C88</f>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F88" s="4">
+        <f>F6*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>2</v>
       </c>
@@ -3836,18 +4375,22 @@
       </c>
       <c r="C89" s="4">
         <f>C7*SimParameters!B10</f>
-        <v>0.15000000000000002</v>
+        <v>0</v>
       </c>
       <c r="D89" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E89" s="4">
-        <f t="shared" ref="E89:E123" si="5">1-C89-D89</f>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+        <f t="shared" ref="E89:E123" si="6">1-C89-D89</f>
+        <v>1</v>
+      </c>
+      <c r="F89" s="4">
+        <f>F7*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>2</v>
       </c>
@@ -3856,18 +4399,22 @@
       </c>
       <c r="C90" s="4">
         <f>C8*SimParameters!B10</f>
-        <v>0.13500000000000001</v>
+        <v>0</v>
       </c>
       <c r="D90" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E90" s="4">
-        <f t="shared" si="5"/>
-        <v>0.86499999999999999</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F90" s="4">
+        <f>F8*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>2</v>
       </c>
@@ -3879,15 +4426,19 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="D91" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E91" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.86499999999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91" s="4">
+        <f>F9*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>2</v>
       </c>
@@ -3899,15 +4450,19 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="D92" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E92" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.97750000000000004</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92" s="4">
+        <f>F10*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>2</v>
       </c>
@@ -3919,15 +4474,19 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="D93" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E93" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.97750000000000004</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93" s="4">
+        <f>F11*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>2</v>
       </c>
@@ -3939,15 +4498,19 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="D94" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E94" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.97750000000000004</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94" s="4">
+        <f>F12*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>2</v>
       </c>
@@ -3959,15 +4522,19 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="D95" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E95" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.97750000000000004</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95" s="4">
+        <f>F13*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>2</v>
       </c>
@@ -3979,15 +4546,19 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D96" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E96" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.98499999999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96" s="4">
+        <f>F14*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>2</v>
       </c>
@@ -3999,15 +4570,19 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D97" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E97" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.98499999999999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97" s="4">
+        <f>F15*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>2</v>
       </c>
@@ -4019,15 +4594,19 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D98" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E98" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.98499999999999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98" s="4">
+        <f>F16*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>2</v>
       </c>
@@ -4039,15 +4618,19 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D99" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E99" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.98499999999999999</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99" s="4">
+        <f>F17*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>2</v>
       </c>
@@ -4059,15 +4642,19 @@
         <v>1.2000000000000001E-3</v>
       </c>
       <c r="D100" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E100" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.99880000000000002</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100" s="4">
+        <f>F18*SimParameters!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>2</v>
       </c>
@@ -4079,15 +4666,19 @@
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="D101" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E101" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.99919999999999998</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101" s="4">
+        <f>F19</f>
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>2</v>
       </c>
@@ -4095,19 +4686,23 @@
         <v>18</v>
       </c>
       <c r="C102" s="4">
-        <f t="shared" ref="C102:C124" si="6">C20</f>
+        <f t="shared" ref="C102:C124" si="7">C20</f>
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="D102" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E102" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.99919999999999998</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102" s="4">
+        <f t="shared" ref="F102:F124" si="8">F20</f>
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>2</v>
       </c>
@@ -4115,19 +4710,23 @@
         <v>19</v>
       </c>
       <c r="C103" s="4">
+        <f t="shared" si="7"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="D103" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E103" s="4">
         <f t="shared" si="6"/>
+        <v>0.99919999999999998</v>
+      </c>
+      <c r="F103" s="4">
+        <f t="shared" si="8"/>
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="D103" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E103" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99919999999999998</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>2</v>
       </c>
@@ -4135,19 +4734,23 @@
         <v>20</v>
       </c>
       <c r="C104" s="4">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D104" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E104" s="4">
         <f t="shared" si="6"/>
+        <v>0.99997499999999995</v>
+      </c>
+      <c r="F104" s="4">
+        <f t="shared" si="8"/>
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="D104" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E104" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99997499999999995</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>2</v>
       </c>
@@ -4155,19 +4758,23 @@
         <v>21</v>
       </c>
       <c r="C105" s="4">
+        <f t="shared" si="7"/>
+        <v>5.9999999999999997E-7</v>
+      </c>
+      <c r="D105" s="4">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E105" s="4">
         <f t="shared" si="6"/>
+        <v>0.99998940000000003</v>
+      </c>
+      <c r="F105" s="4">
+        <f t="shared" si="8"/>
         <v>5.9999999999999997E-7</v>
       </c>
-      <c r="D105" s="4">
-        <f t="shared" si="4"/>
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="E105" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99998940000000003</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>2</v>
       </c>
@@ -4175,19 +4782,23 @@
         <v>22</v>
       </c>
       <c r="C106" s="4">
+        <f t="shared" si="7"/>
+        <v>5.9999999999999997E-7</v>
+      </c>
+      <c r="D106" s="4">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E106" s="4">
         <f t="shared" si="6"/>
+        <v>0.99998940000000003</v>
+      </c>
+      <c r="F106" s="4">
+        <f t="shared" si="8"/>
         <v>5.9999999999999997E-7</v>
       </c>
-      <c r="D106" s="4">
-        <f t="shared" si="4"/>
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="E106" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99998940000000003</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>2</v>
       </c>
@@ -4195,19 +4806,23 @@
         <v>23</v>
       </c>
       <c r="C107" s="4">
+        <f t="shared" si="7"/>
+        <v>5.9999999999999997E-7</v>
+      </c>
+      <c r="D107" s="4">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E107" s="4">
         <f t="shared" si="6"/>
+        <v>0.99998940000000003</v>
+      </c>
+      <c r="F107" s="4">
+        <f t="shared" si="8"/>
         <v>5.9999999999999997E-7</v>
       </c>
-      <c r="D107" s="4">
-        <f t="shared" si="4"/>
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="E107" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99998940000000003</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>2</v>
       </c>
@@ -4215,19 +4830,23 @@
         <v>24</v>
       </c>
       <c r="C108" s="4">
+        <f t="shared" si="7"/>
+        <v>5.9999999999999997E-7</v>
+      </c>
+      <c r="D108" s="4">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="E108" s="4">
         <f t="shared" si="6"/>
+        <v>0.99899939999999998</v>
+      </c>
+      <c r="F108" s="4">
+        <f t="shared" si="8"/>
         <v>5.9999999999999997E-7</v>
       </c>
-      <c r="D108" s="4">
-        <f t="shared" si="4"/>
-        <v>1E-3</v>
-      </c>
-      <c r="E108" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99899939999999998</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>2</v>
       </c>
@@ -4235,19 +4854,23 @@
         <v>25</v>
       </c>
       <c r="C109" s="4">
+        <f t="shared" si="7"/>
+        <v>5.9999999999999997E-7</v>
+      </c>
+      <c r="D109" s="4">
+        <f t="shared" si="5"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="E109" s="4">
         <f t="shared" si="6"/>
+        <v>0.99849940000000004</v>
+      </c>
+      <c r="F109" s="4">
+        <f t="shared" si="8"/>
         <v>5.9999999999999997E-7</v>
       </c>
-      <c r="D109" s="4">
-        <f t="shared" si="4"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="E109" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99849940000000004</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>2</v>
       </c>
@@ -4255,19 +4878,23 @@
         <v>26</v>
       </c>
       <c r="C110" s="4">
+        <f t="shared" si="7"/>
+        <v>5.9999999999999997E-7</v>
+      </c>
+      <c r="D110" s="4">
+        <f t="shared" si="5"/>
+        <v>1.8E-3</v>
+      </c>
+      <c r="E110" s="4">
         <f t="shared" si="6"/>
+        <v>0.99819939999999996</v>
+      </c>
+      <c r="F110" s="4">
+        <f t="shared" si="8"/>
         <v>5.9999999999999997E-7</v>
       </c>
-      <c r="D110" s="4">
-        <f t="shared" si="4"/>
-        <v>1.8E-3</v>
-      </c>
-      <c r="E110" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99819939999999996</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>2</v>
       </c>
@@ -4275,19 +4902,23 @@
         <v>27</v>
       </c>
       <c r="C111" s="4">
+        <f t="shared" si="7"/>
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="D111" s="4">
+        <f t="shared" si="5"/>
+        <v>2E-3</v>
+      </c>
+      <c r="E111" s="4">
         <f t="shared" si="6"/>
+        <v>0.99799400000000005</v>
+      </c>
+      <c r="F111" s="4">
+        <f t="shared" si="8"/>
         <v>6.0000000000000002E-6</v>
       </c>
-      <c r="D111" s="4">
-        <f t="shared" si="4"/>
-        <v>2E-3</v>
-      </c>
-      <c r="E111" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99799400000000005</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>2</v>
       </c>
@@ -4295,19 +4926,23 @@
         <v>28</v>
       </c>
       <c r="C112" s="4">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D112" s="4">
+        <f t="shared" si="5"/>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E112" s="4">
         <f t="shared" si="6"/>
+        <v>0.99697499999999994</v>
+      </c>
+      <c r="F112" s="4">
+        <f t="shared" si="8"/>
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="D112" s="4">
-        <f t="shared" si="4"/>
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E112" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99697499999999994</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>2</v>
       </c>
@@ -4315,19 +4950,23 @@
         <v>29</v>
       </c>
       <c r="C113" s="4">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D113" s="4">
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E113" s="4">
         <f t="shared" si="6"/>
+        <v>0.99497499999999994</v>
+      </c>
+      <c r="F113" s="4">
+        <f t="shared" si="8"/>
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="D113" s="4">
-        <f t="shared" si="4"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E113" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99497499999999994</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>2</v>
       </c>
@@ -4335,19 +4974,23 @@
         <v>30</v>
       </c>
       <c r="C114" s="4">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D114" s="4">
+        <f t="shared" si="5"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E114" s="4">
         <f t="shared" si="6"/>
+        <v>0.99397499999999994</v>
+      </c>
+      <c r="F114" s="4">
+        <f t="shared" si="8"/>
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="D114" s="4">
-        <f t="shared" si="4"/>
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="E114" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99397499999999994</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>2</v>
       </c>
@@ -4355,19 +4998,23 @@
         <v>31</v>
       </c>
       <c r="C115" s="4">
+        <f t="shared" si="7"/>
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="D115" s="4">
+        <f t="shared" si="5"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E115" s="4">
         <f t="shared" si="6"/>
+        <v>0.99185000000000001</v>
+      </c>
+      <c r="F115" s="4">
+        <f t="shared" si="8"/>
         <v>1.4999999999999999E-4</v>
       </c>
-      <c r="D115" s="4">
-        <f t="shared" si="4"/>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="E115" s="4">
-        <f t="shared" si="5"/>
-        <v>0.99185000000000001</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>2</v>
       </c>
@@ -4375,19 +5022,23 @@
         <v>32</v>
       </c>
       <c r="C116" s="4">
+        <f t="shared" si="7"/>
+        <v>3.5E-4</v>
+      </c>
+      <c r="D116" s="4">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="E116" s="4">
         <f t="shared" si="6"/>
+        <v>0.94964999999999999</v>
+      </c>
+      <c r="F116" s="4">
+        <f t="shared" si="8"/>
         <v>3.5E-4</v>
       </c>
-      <c r="D116" s="4">
-        <f t="shared" si="4"/>
-        <v>0.05</v>
-      </c>
-      <c r="E116" s="4">
-        <f t="shared" si="5"/>
-        <v>0.94964999999999999</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>2</v>
       </c>
@@ -4395,19 +5046,23 @@
         <v>33</v>
       </c>
       <c r="C117" s="4">
+        <f t="shared" si="7"/>
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="D117" s="4">
+        <f t="shared" si="5"/>
+        <v>0.08</v>
+      </c>
+      <c r="E117" s="4">
         <f t="shared" si="6"/>
+        <v>0.91944999999999999</v>
+      </c>
+      <c r="F117" s="4">
+        <f t="shared" si="8"/>
         <v>5.5000000000000003E-4</v>
       </c>
-      <c r="D117" s="4">
-        <f t="shared" si="4"/>
-        <v>0.08</v>
-      </c>
-      <c r="E117" s="4">
-        <f t="shared" si="5"/>
-        <v>0.91944999999999999</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>2</v>
       </c>
@@ -4415,19 +5070,23 @@
         <v>34</v>
       </c>
       <c r="C118" s="4">
+        <f t="shared" si="7"/>
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="D118" s="4">
+        <f t="shared" si="5"/>
+        <v>0.35</v>
+      </c>
+      <c r="E118" s="4">
         <f t="shared" si="6"/>
+        <v>0.64650000000000007</v>
+      </c>
+      <c r="F118" s="4">
+        <f t="shared" si="8"/>
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="D118" s="4">
-        <f t="shared" si="4"/>
-        <v>0.35</v>
-      </c>
-      <c r="E118" s="4">
-        <f t="shared" si="5"/>
-        <v>0.64650000000000007</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>2</v>
       </c>
@@ -4435,19 +5094,23 @@
         <v>35</v>
       </c>
       <c r="C119" s="4">
+        <f t="shared" si="7"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="D119" s="4">
+        <f t="shared" si="5"/>
+        <v>0.4</v>
+      </c>
+      <c r="E119" s="4">
         <f t="shared" si="6"/>
+        <v>0.59850000000000003</v>
+      </c>
+      <c r="F119" s="4">
+        <f t="shared" si="8"/>
         <v>1.5E-3</v>
       </c>
-      <c r="D119" s="4">
-        <f t="shared" si="4"/>
-        <v>0.4</v>
-      </c>
-      <c r="E119" s="4">
-        <f t="shared" si="5"/>
-        <v>0.59850000000000003</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>2</v>
       </c>
@@ -4455,19 +5118,23 @@
         <v>36</v>
       </c>
       <c r="C120" s="4">
+        <f t="shared" si="7"/>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D120" s="4">
+        <f t="shared" si="5"/>
+        <v>0.7</v>
+      </c>
+      <c r="E120" s="4">
         <f t="shared" si="6"/>
+        <v>0.2984</v>
+      </c>
+      <c r="F120" s="4">
+        <f t="shared" si="8"/>
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="D120" s="4">
-        <f t="shared" si="4"/>
-        <v>0.7</v>
-      </c>
-      <c r="E120" s="4">
-        <f t="shared" si="5"/>
-        <v>0.2984</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>2</v>
       </c>
@@ -4475,19 +5142,23 @@
         <v>37</v>
       </c>
       <c r="C121" s="4">
+        <f t="shared" si="7"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D121" s="4">
+        <f t="shared" si="5"/>
+        <v>0.7</v>
+      </c>
+      <c r="E121" s="4">
         <f t="shared" si="6"/>
+        <v>0.29400000000000004</v>
+      </c>
+      <c r="F121" s="4">
+        <f t="shared" si="8"/>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D121" s="4">
-        <f t="shared" si="4"/>
-        <v>0.7</v>
-      </c>
-      <c r="E121" s="4">
-        <f t="shared" si="5"/>
-        <v>0.29400000000000004</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
         <v>2</v>
       </c>
@@ -4495,19 +5166,23 @@
         <v>38</v>
       </c>
       <c r="C122" s="4">
+        <f t="shared" si="7"/>
+        <v>0.01</v>
+      </c>
+      <c r="D122" s="4">
+        <f t="shared" si="5"/>
+        <v>0.85</v>
+      </c>
+      <c r="E122" s="4">
         <f t="shared" si="6"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F122" s="4">
+        <f t="shared" si="8"/>
         <v>0.01</v>
       </c>
-      <c r="D122" s="4">
-        <f t="shared" si="4"/>
-        <v>0.85</v>
-      </c>
-      <c r="E122" s="4">
-        <f t="shared" si="5"/>
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>2</v>
       </c>
@@ -4515,19 +5190,23 @@
         <v>39</v>
       </c>
       <c r="C123" s="4">
+        <f t="shared" si="7"/>
+        <v>0.2</v>
+      </c>
+      <c r="D123" s="4">
+        <f t="shared" si="5"/>
+        <v>0.7</v>
+      </c>
+      <c r="E123" s="4">
         <f t="shared" si="6"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="F123" s="4">
+        <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
-      <c r="D123" s="4">
-        <f t="shared" si="4"/>
-        <v>0.7</v>
-      </c>
-      <c r="E123" s="4">
-        <f t="shared" si="5"/>
-        <v>0.10000000000000009</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>2</v>
       </c>
@@ -4535,15 +5214,19 @@
         <v>40</v>
       </c>
       <c r="C124" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.2</v>
       </c>
       <c r="D124" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.8</v>
       </c>
       <c r="E124" s="4">
         <v>0</v>
+      </c>
+      <c r="F124" s="4">
+        <f t="shared" si="8"/>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -4594,7 +5277,7 @@
       </c>
       <c r="C2" s="2">
         <f>potential_preg_untrt!C2*SimParameters!B3</f>
-        <v>6.9999999999999993E-2</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2">
         <f>potential_preg_untrt!D2</f>
@@ -4602,7 +5285,7 @@
       </c>
       <c r="E2" s="2">
         <f>1-D2-C2</f>
-        <v>0.93</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -4614,7 +5297,7 @@
       </c>
       <c r="C3" s="2">
         <f>potential_preg_untrt!C3*SimParameters!B3</f>
-        <v>6.9999999999999993E-2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
         <f>potential_preg_untrt!D3</f>
@@ -4622,7 +5305,7 @@
       </c>
       <c r="E3" s="2">
         <f>1-D3-C3</f>
-        <v>0.93</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -4634,7 +5317,7 @@
       </c>
       <c r="C4" s="2">
         <f>potential_preg_untrt!C4*SimParameters!B3</f>
-        <v>3.4999999999999996E-2</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <f>potential_preg_untrt!D4</f>
@@ -4642,7 +5325,7 @@
       </c>
       <c r="E4" s="2">
         <f>1-D4-C4</f>
-        <v>0.96499999999999997</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -4654,7 +5337,7 @@
       </c>
       <c r="C5" s="2">
         <f>potential_preg_untrt!C5*SimParameters!B3</f>
-        <v>3.4999999999999996E-2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2">
         <f>potential_preg_untrt!D5</f>
@@ -4662,7 +5345,7 @@
       </c>
       <c r="E5" s="2">
         <f>1-D5-C5</f>
-        <v>0.96499999999999997</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -4674,7 +5357,7 @@
       </c>
       <c r="C6" s="2">
         <f>potential_preg_untrt!C6*SimParameters!B3</f>
-        <v>6.9999999999999993E-2</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <f>potential_preg_untrt!D6</f>
@@ -4682,7 +5365,7 @@
       </c>
       <c r="E6" s="2">
         <f>1-D6-C6</f>
-        <v>0.93</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -4694,7 +5377,7 @@
       </c>
       <c r="C7" s="2">
         <f>potential_preg_untrt!C7*SimParameters!B3</f>
-        <v>6.9999999999999993E-2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
         <f>potential_preg_untrt!D7</f>
@@ -4702,7 +5385,7 @@
       </c>
       <c r="E7" s="2">
         <f t="shared" ref="E7:E41" si="0">1-C7-D7</f>
-        <v>0.93</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -4714,7 +5397,7 @@
       </c>
       <c r="C8" s="2">
         <f>potential_preg_untrt!C8*SimParameters!B3</f>
-        <v>6.3E-2</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2">
         <f>potential_preg_untrt!D8</f>
@@ -4722,7 +5405,7 @@
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>0.93700000000000006</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -5413,7 +6096,7 @@
       </c>
       <c r="C43" s="3">
         <f>potential_preg_untrt!C43*SimParameters!$B$3</f>
-        <v>8.7499999999999994E-2</v>
+        <v>0</v>
       </c>
       <c r="D43" s="3">
         <f>potential_preg_untrt!D43</f>
@@ -5421,7 +6104,7 @@
       </c>
       <c r="E43" s="3">
         <f>1-D43-C43</f>
-        <v>0.91249999999999998</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -5433,7 +6116,7 @@
       </c>
       <c r="C44" s="3">
         <f>potential_preg_untrt!C44*SimParameters!$B$3</f>
-        <v>8.7499999999999994E-2</v>
+        <v>0</v>
       </c>
       <c r="D44" s="3">
         <f>potential_preg_untrt!D44</f>
@@ -5441,7 +6124,7 @@
       </c>
       <c r="E44" s="3">
         <f>1-D44-C44</f>
-        <v>0.91249999999999998</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -5453,7 +6136,7 @@
       </c>
       <c r="C45" s="3">
         <f>potential_preg_untrt!C45*SimParameters!$B$3</f>
-        <v>4.3749999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="D45" s="3">
         <f>potential_preg_untrt!D45</f>
@@ -5461,7 +6144,7 @@
       </c>
       <c r="E45" s="3">
         <f>1-D45-C45</f>
-        <v>0.95625000000000004</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -5473,7 +6156,7 @@
       </c>
       <c r="C46" s="3">
         <f>potential_preg_untrt!C46*SimParameters!$B$3</f>
-        <v>4.3749999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="D46" s="3">
         <f>potential_preg_untrt!D46</f>
@@ -5481,7 +6164,7 @@
       </c>
       <c r="E46" s="3">
         <f>1-D46-C46</f>
-        <v>0.95625000000000004</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -5493,7 +6176,7 @@
       </c>
       <c r="C47" s="3">
         <f>potential_preg_untrt!C47*SimParameters!$B$3</f>
-        <v>8.7499999999999994E-2</v>
+        <v>0</v>
       </c>
       <c r="D47" s="3">
         <f>potential_preg_untrt!D47</f>
@@ -5501,7 +6184,7 @@
       </c>
       <c r="E47" s="3">
         <f>1-D47-C47</f>
-        <v>0.91249999999999998</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -5513,7 +6196,7 @@
       </c>
       <c r="C48" s="3">
         <f>potential_preg_untrt!C48*SimParameters!$B$3</f>
-        <v>8.7499999999999994E-2</v>
+        <v>0</v>
       </c>
       <c r="D48" s="3">
         <f>potential_preg_untrt!D48</f>
@@ -5521,7 +6204,7 @@
       </c>
       <c r="E48" s="3">
         <f t="shared" ref="E48:E82" si="1">1-C48-D48</f>
-        <v>0.91249999999999998</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -5533,7 +6216,7 @@
       </c>
       <c r="C49" s="3">
         <f>potential_preg_untrt!C49*SimParameters!$B$3</f>
-        <v>7.8749999999999987E-2</v>
+        <v>0</v>
       </c>
       <c r="D49" s="3">
         <f>potential_preg_untrt!D49</f>
@@ -5541,7 +6224,7 @@
       </c>
       <c r="E49" s="3">
         <f t="shared" si="1"/>
-        <v>0.92125000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -6232,7 +6915,7 @@
       </c>
       <c r="C84" s="4">
         <f>potential_preg_untrt!C84*SimParameters!$B$3</f>
-        <v>0.10500000000000001</v>
+        <v>0</v>
       </c>
       <c r="D84" s="4">
         <f>potential_preg_untrt!D84</f>
@@ -6240,7 +6923,7 @@
       </c>
       <c r="E84" s="4">
         <f>1-D84-C84</f>
-        <v>0.89500000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -6252,7 +6935,7 @@
       </c>
       <c r="C85" s="4">
         <f>potential_preg_untrt!C85*SimParameters!$B$3</f>
-        <v>0.10500000000000001</v>
+        <v>0</v>
       </c>
       <c r="D85" s="4">
         <f>potential_preg_untrt!D85</f>
@@ -6260,7 +6943,7 @@
       </c>
       <c r="E85" s="4">
         <f>1-D85-C85</f>
-        <v>0.89500000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -6272,7 +6955,7 @@
       </c>
       <c r="C86" s="4">
         <f>potential_preg_untrt!C86*SimParameters!$B$3</f>
-        <v>5.2500000000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="D86" s="4">
         <f>potential_preg_untrt!D86</f>
@@ -6280,7 +6963,7 @@
       </c>
       <c r="E86" s="4">
         <f>1-D86-C86</f>
-        <v>0.94750000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -6292,7 +6975,7 @@
       </c>
       <c r="C87" s="4">
         <f>potential_preg_untrt!C87*SimParameters!$B$3</f>
-        <v>5.2500000000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="D87" s="4">
         <f>potential_preg_untrt!D87</f>
@@ -6300,7 +6983,7 @@
       </c>
       <c r="E87" s="4">
         <f>1-D87-C87</f>
-        <v>0.94750000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -6312,7 +6995,7 @@
       </c>
       <c r="C88" s="4">
         <f>potential_preg_untrt!C88*SimParameters!$B$3</f>
-        <v>0.10500000000000001</v>
+        <v>0</v>
       </c>
       <c r="D88" s="4">
         <f>potential_preg_untrt!D88</f>
@@ -6320,7 +7003,7 @@
       </c>
       <c r="E88" s="4">
         <f>1-D88-C88</f>
-        <v>0.89500000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -6332,7 +7015,7 @@
       </c>
       <c r="C89" s="4">
         <f>potential_preg_untrt!C89*SimParameters!$B$3</f>
-        <v>0.10500000000000001</v>
+        <v>0</v>
       </c>
       <c r="D89" s="4">
         <f>potential_preg_untrt!D89</f>
@@ -6340,7 +7023,7 @@
       </c>
       <c r="E89" s="4">
         <f t="shared" ref="E89:E123" si="2">1-C89-D89</f>
-        <v>0.89500000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -6352,7 +7035,7 @@
       </c>
       <c r="C90" s="4">
         <f>potential_preg_untrt!C90*SimParameters!$B$3</f>
-        <v>9.4500000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="D90" s="4">
         <f>potential_preg_untrt!D90</f>
@@ -6360,7 +7043,7 @@
       </c>
       <c r="E90" s="4">
         <f t="shared" si="2"/>
-        <v>0.90549999999999997</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -15422,6 +16105,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -15646,16 +16338,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15672,12 +16363,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>